<commit_message>
added styling and started OAuth2 implementation
</commit_message>
<xml_diff>
--- a/ngToDo/Server/ExcelWorkbook-DataSource/ngToDo.xlsx
+++ b/ngToDo/Server/ExcelWorkbook-DataSource/ngToDo.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17985" windowHeight="6638"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17985" windowHeight="6638" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ToDos" sheetId="1" r:id="rId1"/>
+    <sheet name="Users" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Id</t>
   </si>
@@ -51,6 +52,21 @@
   </si>
   <si>
     <t>To Do App</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Firstname</t>
+  </si>
+  <si>
+    <t>Lastname</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
   </si>
 </sst>
 </file>
@@ -370,7 +386,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -423,4 +439,42 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat(add oauth2 enabled login)
</commit_message>
<xml_diff>
--- a/ngToDo/Server/ExcelWorkbook-DataSource/ngToDo.xlsx
+++ b/ngToDo/Server/ExcelWorkbook-DataSource/ngToDo.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Id</t>
   </si>
@@ -67,16 +67,36 @@
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>P@ssw0rd</t>
+  </si>
+  <si>
+    <t>Quinntyne</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>quinntynebrown@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -99,13 +119,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -443,13 +466,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="20" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="5.59765625" customWidth="1"/>
+    <col min="2" max="2" width="28.06640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
@@ -474,7 +501,35 @@
         <v>6</v>
       </c>
     </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId2"/>
+    <hyperlink ref="F2" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>